<commit_message>
Setup playwright tests + shakeout e2e test
</commit_message>
<xml_diff>
--- a/NearBeach/tests/Template of Unit Tests.xlsx
+++ b/NearBeach/tests/Template of Unit Tests.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke/Sites/NearBeach/NearBeach/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D94AE22-449F-7045-A3E0-699E0DD92CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5386CDB-1D71-3E41-9991-16B3609A444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{49CA0490-8A4C-AD4D-8E45-19DFC0D521BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{49CA0490-8A4C-AD4D-8E45-19DFC0D521BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="URLS" sheetId="2" r:id="rId3"/>
+    <sheet name="Play Wright" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">URLS!$A$1:$J$164</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="677">
   <si>
     <t>AddBugForm</t>
   </si>
@@ -1847,6 +1848,231 @@
   </si>
   <si>
     <t>{"rfc_title":"Simple RFC Title","rfc_summary":"Simple RFC Summary","rfc_type":1,"rfc_implementation_start_date":0,"rfc_implementation_end_date":0,"rfc_implementation_release_date":0,"rfc_version_number":"0.30.0","rfc_lead":1,"rfc_priority":1,"rfc_risk":1,"rfc_impact":"Risk Impact","rfc_risk_and_impact_analysis":"Impact Analysis","rfc_implementation_plan":"Implementation Plan","rfc_backout_plan":"Backout Plan","rfc_test_plan":"Test PLan","group_list":[1,2]}</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>Test Url</t>
+  </si>
+  <si>
+    <t>Test Page Title</t>
+  </si>
+  <si>
+    <t>Test Page Heading</t>
+  </si>
+  <si>
+    <t>Screenshot Path</t>
+  </si>
+  <si>
+    <t>Card Information 1</t>
+  </si>
+  <si>
+    <t>Change Task Information 1</t>
+  </si>
+  <si>
+    <t>Customer Information 1</t>
+  </si>
+  <si>
+    <t>Group Information 1</t>
+  </si>
+  <si>
+    <t>Kanban Information 1</t>
+  </si>
+  <si>
+    <t>Kanban Card Information 1</t>
+  </si>
+  <si>
+    <t>Kanban Information Edit Board 1</t>
+  </si>
+  <si>
+    <t>New Group</t>
+  </si>
+  <si>
+    <t>New Kanban</t>
+  </si>
+  <si>
+    <t>New Organisation</t>
+  </si>
+  <si>
+    <t>New Permission Set</t>
+  </si>
+  <si>
+    <t>New Project</t>
+  </si>
+  <si>
+    <t>New Request for Change</t>
+  </si>
+  <si>
+    <t>New Requirement Item</t>
+  </si>
+  <si>
+    <t>New Requirement</t>
+  </si>
+  <si>
+    <t>New Task</t>
+  </si>
+  <si>
+    <t>New User</t>
+  </si>
+  <si>
+    <t>Organisation Information</t>
+  </si>
+  <si>
+    <t>Organisation Information 1</t>
+  </si>
+  <si>
+    <t>Permission Set Information 1</t>
+  </si>
+  <si>
+    <t>Profile Information</t>
+  </si>
+  <si>
+    <t>Project Information 1</t>
+  </si>
+  <si>
+    <t>Requirement Information 1</t>
+  </si>
+  <si>
+    <t>Requirement Item Information 1</t>
+  </si>
+  <si>
+    <t>RFC Information 1</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Task Information 1</t>
+  </si>
+  <si>
+    <t>User Information 1</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_group/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_kanban/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_organisation/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_permission_set/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_project/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_request_for_change/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_requirement/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_task/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_user/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/profile_information/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/search/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/card_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/change_task_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/customer_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/group_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/kanban_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/kanban_information/1/card/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/kanban_information/1/edit_board/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/new_requirement_item/save/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/organisation_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/permission_set_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/project_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/requirement_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/requirement_item_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/rfc_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/task_information/1/</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/user_information/1/</t>
+  </si>
+  <si>
+    <t>Change Task 1</t>
+  </si>
+  <si>
+    <t>Kanban Information</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Change Task</t>
+  </si>
+  <si>
+    <t>Customer Information</t>
+  </si>
+  <si>
+    <t>Group Information</t>
+  </si>
+  <si>
+    <t>Permission Set Information</t>
+  </si>
+  <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Requirement Information</t>
+  </si>
+  <si>
+    <t>Requirement Item Information</t>
+  </si>
+  <si>
+    <t>RFC Information</t>
+  </si>
+  <si>
+    <t>Task Information</t>
+  </si>
+  <si>
+    <t>User Information</t>
   </si>
 </sst>
 </file>
@@ -2827,10 +3053,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B713DD-523F-5F48-9EE2-FA87D0BABFC5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C58" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2911,7 +3138,7 @@
         <v>URLTest('dashboard', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -2946,7 +3173,7 @@
         <v>URLTest('admin_add_user', [], {"username":2}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
@@ -3042,7 +3269,7 @@
         <v>URLTest('change_task_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -3074,7 +3301,7 @@
         <v>URLTest('change_task_delete', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -3106,7 +3333,7 @@
         <v>URLTest('change_task_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>79</v>
       </c>
@@ -3170,7 +3397,7 @@
         <v>URLTest('customer_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>83</v>
       </c>
@@ -3202,7 +3429,7 @@
         <v>URLTest('customer_get_profile_image', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -3234,7 +3461,7 @@
         <v>URLTest('customer_update_profile', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -3266,7 +3493,7 @@
         <v>URLTest('customer_information_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
@@ -3298,7 +3525,7 @@
         <v>URLTest('get_bug_list', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>91</v>
       </c>
@@ -3330,7 +3557,7 @@
         <v>URLTest('get_kanban_list', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>93</v>
       </c>
@@ -3362,7 +3589,7 @@
         <v>URLTest('get_my_objects', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>95</v>
       </c>
@@ -3394,7 +3621,7 @@
         <v>URLTest('rfc_approvals', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
@@ -3426,7 +3653,7 @@
         <v>URLTest('get_unassigned_objects', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>99</v>
       </c>
@@ -3458,7 +3685,7 @@
         <v>URLTest('users_with_no_groups', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>101</v>
       </c>
@@ -3487,7 +3714,7 @@
         <v>URLTest('document_add_folder', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>103</v>
       </c>
@@ -3516,7 +3743,7 @@
         <v>URLTest('document_add_link', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>105</v>
       </c>
@@ -3545,7 +3772,7 @@
         <v>URLTest('document_list_files', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>107</v>
       </c>
@@ -3574,7 +3801,7 @@
         <v>URLTest('document_list_folders', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>109</v>
       </c>
@@ -3603,7 +3830,7 @@
         <v>URLTest('document_upload', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>111</v>
       </c>
@@ -3667,7 +3894,7 @@
         <v>URLTest('group_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>115</v>
       </c>
@@ -3699,7 +3926,7 @@
         <v>URLTest('group_information_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>117</v>
       </c>
@@ -3731,7 +3958,7 @@
         <v>URLTest('check_group_name', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>119</v>
       </c>
@@ -3763,7 +3990,7 @@
         <v>URLTest('kanban_edit_column', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>121</v>
       </c>
@@ -3795,7 +4022,7 @@
         <v>URLTest('kanban_delete_column', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>123</v>
       </c>
@@ -3827,7 +4054,7 @@
         <v>URLTest('kanban_new_column', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>125</v>
       </c>
@@ -3859,7 +4086,7 @@
         <v>URLTest('kanban_resort_column', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>127</v>
       </c>
@@ -3891,7 +4118,7 @@
         <v>URLTest('kanban_edit_level', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>129</v>
       </c>
@@ -3923,7 +4150,7 @@
         <v>URLTest('kanban_delete_level', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>131</v>
       </c>
@@ -3955,7 +4182,7 @@
         <v>URLTest('kanban_new_level', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>133</v>
       </c>
@@ -3987,7 +4214,7 @@
         <v>URLTest('kanban_resort_level', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>135</v>
       </c>
@@ -4083,7 +4310,7 @@
         <v>URLTest('kanban_information', [1,1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>140</v>
       </c>
@@ -4147,7 +4374,7 @@
         <v>URLTest('kanban_edit_board', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>144</v>
       </c>
@@ -4179,7 +4406,7 @@
         <v>URLTest('add_kanban_link', [1,1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
@@ -4211,7 +4438,7 @@
         <v>URLTest('kanban_link_list', [1,1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>148</v>
       </c>
@@ -4243,7 +4470,7 @@
         <v>URLTest('new_kanban_card', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>150</v>
       </c>
@@ -4275,7 +4502,7 @@
         <v>URLTest('move_kanban_card', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>152</v>
       </c>
@@ -4307,7 +4534,7 @@
         <v>URLTest('check_kanban_board_name', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>154</v>
       </c>
@@ -4435,7 +4662,7 @@
         <v>URLTest('permission_set_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>162</v>
       </c>
@@ -4467,7 +4694,7 @@
         <v>URLTest('permission_set_information_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>164</v>
       </c>
@@ -4531,7 +4758,7 @@
         <v>URLTest('profile_information', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>168</v>
       </c>
@@ -4563,7 +4790,7 @@
         <v>URLTest('profile_update_data', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>170</v>
       </c>
@@ -4595,7 +4822,7 @@
         <v>URLTest('profile_update_profile', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>172</v>
       </c>
@@ -4627,7 +4854,7 @@
         <v>URLTest('new_customer', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>174</v>
       </c>
@@ -4691,7 +4918,7 @@
         <v>URLTest('new_group', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>178</v>
       </c>
@@ -4755,7 +4982,7 @@
         <v>URLTest('new_kanban', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>182</v>
       </c>
@@ -4819,7 +5046,7 @@
         <v>URLTest('new_organisation', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>186</v>
       </c>
@@ -4883,7 +5110,7 @@
         <v>URLTest('new_permission_set', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>190</v>
       </c>
@@ -4947,7 +5174,7 @@
         <v>URLTest('new_project', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>194</v>
       </c>
@@ -5011,7 +5238,7 @@
         <v>URLTest('new_request_for_change', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>198</v>
       </c>
@@ -5075,7 +5302,7 @@
         <v>URLTest('new_requirement', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>202</v>
       </c>
@@ -5174,7 +5401,7 @@
         <v>URLTest('new_task', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>208</v>
       </c>
@@ -5238,7 +5465,7 @@
         <v>URLTest('new_user', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>212</v>
       </c>
@@ -5270,7 +5497,7 @@
         <v>URLTest('new_user_save', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>214</v>
       </c>
@@ -5302,7 +5529,7 @@
         <v>URLTest('admin_add_user', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>215</v>
       </c>
@@ -5331,7 +5558,7 @@
         <v>URLTest('add_bug', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>217</v>
       </c>
@@ -5366,7 +5593,7 @@
         <v>URLTest('add_customer', ["project",1], {"customer":1}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>219</v>
       </c>
@@ -5401,7 +5628,7 @@
         <v>URLTest('add_group', ["project",1], {"group_list": [1,2]}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>221</v>
       </c>
@@ -5433,7 +5660,7 @@
         <v>URLTest('add_link', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>223</v>
       </c>
@@ -5468,7 +5695,7 @@
         <v>URLTest('add_notes', ["project",1], {"note":"A simple note"}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>225</v>
       </c>
@@ -5503,7 +5730,7 @@
         <v>URLTest('add_tags', ["project",1], {"tag":1}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>227</v>
       </c>
@@ -5538,7 +5765,7 @@
         <v>URLTest('add_user', ["project",1], {"username":2}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>229</v>
       </c>
@@ -5570,7 +5797,7 @@
         <v>URLTest('associated_objects', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>231</v>
       </c>
@@ -5602,7 +5829,7 @@
         <v>URLTest('bug_client_list', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>233</v>
       </c>
@@ -5634,7 +5861,7 @@
         <v>URLTest('bug_list', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>235</v>
       </c>
@@ -5666,7 +5893,7 @@
         <v>URLTest('customer_list', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>237</v>
       </c>
@@ -5698,7 +5925,7 @@
         <v>URLTest('customer_list_all', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>239</v>
       </c>
@@ -5730,7 +5957,7 @@
         <v>URLTest('group_list', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>241</v>
       </c>
@@ -5762,7 +5989,7 @@
         <v>URLTest('group_list_all', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>243</v>
       </c>
@@ -5791,7 +6018,7 @@
         <v>URLTest('link_list', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>245</v>
       </c>
@@ -5823,7 +6050,7 @@
         <v>URLTest('note_list', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>247</v>
       </c>
@@ -5855,7 +6082,7 @@
         <v>URLTest('object_link_list', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>249</v>
       </c>
@@ -5890,7 +6117,7 @@
         <v>URLTest('query_bug_client', ["project",1], 0, 200,'POST'),</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>251</v>
       </c>
@@ -5925,7 +6152,7 @@
         <v>URLTest('remove_group', ["project",1], 0, 200,'POST'),</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>253</v>
       </c>
@@ -5960,7 +6187,7 @@
         <v>URLTest('remove_link', ["project",1], 0, 200,'POST'),</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>255</v>
       </c>
@@ -5995,7 +6222,7 @@
         <v>URLTest('remove_user', ["project",1], 0, 200,'POST'),</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>257</v>
       </c>
@@ -6027,7 +6254,7 @@
         <v>URLTest('tag_list', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>259</v>
       </c>
@@ -6059,7 +6286,7 @@
         <v>URLTest('tag_list_all', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>261</v>
       </c>
@@ -6091,7 +6318,7 @@
         <v>URLTest('user_list', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>263</v>
       </c>
@@ -6123,7 +6350,7 @@
         <v>URLTest('user_list_all', ["project",1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>265</v>
       </c>
@@ -6155,7 +6382,7 @@
         <v>URLTest('delete_bug', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>267</v>
       </c>
@@ -6187,7 +6414,7 @@
         <v>URLTest('delete_link', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>269</v>
       </c>
@@ -6219,7 +6446,7 @@
         <v>URLTest('delete_tag', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>271</v>
       </c>
@@ -6251,7 +6478,7 @@
         <v>URLTest('lead_user_list', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>273</v>
       </c>
@@ -6315,7 +6542,7 @@
         <v>URLTest('organisation_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>277</v>
       </c>
@@ -6347,7 +6574,7 @@
         <v>URLTest('organisation_get_profile_picture', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>279</v>
       </c>
@@ -6379,7 +6606,7 @@
         <v>URLTest('organisation_information_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>281</v>
       </c>
@@ -6443,7 +6670,7 @@
         <v>URLTest('project_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>285</v>
       </c>
@@ -6507,7 +6734,7 @@
         <v>URLTest('requirement_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>289</v>
       </c>
@@ -6539,7 +6766,7 @@
         <v>URLTest('add_requirement_link', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>291</v>
       </c>
@@ -6571,7 +6798,7 @@
         <v>URLTest('get_requirement_item_links', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>293</v>
       </c>
@@ -6603,7 +6830,7 @@
         <v>URLTest('get_requirement_items', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>295</v>
       </c>
@@ -6635,7 +6862,7 @@
         <v>URLTest('get_requirement_item_status_list', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>297</v>
       </c>
@@ -6667,7 +6894,7 @@
         <v>URLTest('get_requirement_item_type_list', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>299</v>
       </c>
@@ -6699,7 +6926,7 @@
         <v>URLTest('get_requirement_links_list', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>301</v>
       </c>
@@ -6763,7 +6990,7 @@
         <v>URLTest('requirement_item_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>305</v>
       </c>
@@ -6827,7 +7054,7 @@
         <v>URLTest('requirement_item_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>307</v>
       </c>
@@ -6859,7 +7086,7 @@
         <v>URLTest('get_requirement_item_links_list', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>309</v>
       </c>
@@ -6891,7 +7118,7 @@
         <v>URLTest('requirement_information_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>310</v>
       </c>
@@ -6955,7 +7182,7 @@
         <v>URLTest('rfc_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>314</v>
       </c>
@@ -6987,7 +7214,7 @@
         <v>URLTest('rfc_change_task_list', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>316</v>
       </c>
@@ -7019,7 +7246,7 @@
         <v>URLTest('rfc_new_change_task', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>318</v>
       </c>
@@ -7051,7 +7278,7 @@
         <v>URLTest('rfc_information_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>320</v>
       </c>
@@ -7083,7 +7310,7 @@
         <v>URLTest('rfc_save_backout', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>322</v>
       </c>
@@ -7115,7 +7342,7 @@
         <v>URLTest('rfc_save_implementation', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>324</v>
       </c>
@@ -7147,7 +7374,7 @@
         <v>URLTest('rfc_save_risk', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>326</v>
       </c>
@@ -7179,7 +7406,7 @@
         <v>URLTest('rfc_save_test', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>328</v>
       </c>
@@ -7211,7 +7438,7 @@
         <v>URLTest('rfc_update_status', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>330</v>
       </c>
@@ -7275,7 +7502,7 @@
         <v>URLTest('search', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>334</v>
       </c>
@@ -7307,7 +7534,7 @@
         <v>URLTest('search_data', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>336</v>
       </c>
@@ -7339,7 +7566,7 @@
         <v>URLTest('search_group', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>338</v>
       </c>
@@ -7371,7 +7598,7 @@
         <v>URLTest('search_group_data', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>340</v>
       </c>
@@ -7403,7 +7630,7 @@
         <v>URLTest('search_customer', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>342</v>
       </c>
@@ -7435,7 +7662,7 @@
         <v>URLTest('search_customer_data', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>344</v>
       </c>
@@ -7467,7 +7694,7 @@
         <v>URLTest('search_organisation', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>346</v>
       </c>
@@ -7499,7 +7726,7 @@
         <v>URLTest('search_organisation_data', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>348</v>
       </c>
@@ -7531,7 +7758,7 @@
         <v>URLTest('search_permission_set', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>350</v>
       </c>
@@ -7563,7 +7790,7 @@
         <v>URLTest('search_permission_set_data', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>352</v>
       </c>
@@ -7595,7 +7822,7 @@
         <v>URLTest('search_tag', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>354</v>
       </c>
@@ -7627,7 +7854,7 @@
         <v>URLTest('search_user', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>356</v>
       </c>
@@ -7659,7 +7886,7 @@
         <v>URLTest('search_user_data', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>358</v>
       </c>
@@ -7691,7 +7918,7 @@
         <v>URLTest('delete_tag', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>359</v>
       </c>
@@ -7723,7 +7950,7 @@
         <v>URLTest('new_tag', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>361</v>
       </c>
@@ -7787,7 +8014,7 @@
         <v>URLTest('task_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>365</v>
       </c>
@@ -7851,7 +8078,7 @@
         <v>URLTest('user_information', [1], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>369</v>
       </c>
@@ -7883,7 +8110,7 @@
         <v>URLTest('user_information_save', [1], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>371</v>
       </c>
@@ -7915,7 +8142,7 @@
         <v>URLTest('update_password', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>373</v>
       </c>
@@ -7947,7 +8174,7 @@
         <v>URLTest('test_permission_denied', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>375</v>
       </c>
@@ -8011,7 +8238,7 @@
         <v>URLTest('password_reset', [], {}, 200,'GET'),</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>379</v>
       </c>
@@ -8043,7 +8270,7 @@
         <v>URLTest('password_reset_done', [], {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>381</v>
       </c>
@@ -8072,7 +8299,7 @@
         <v>URLTest('password_reset_confirm', , {}, 200,'POST'),</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>383</v>
       </c>
@@ -8105,7 +8332,839 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J164" xr:uid="{89B713DD-523F-5F48-9EE2-FA87D0BABFC5}"/>
+  <autoFilter ref="A1:J164" xr:uid="{89B713DD-523F-5F48-9EE2-FA87D0BABFC5}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="GET"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8E9096-775A-FD45-9978-9A3BD393E5D5}">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="84.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="193.33203125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>CONCATENATE("./test-results/",F2,".jpg")</f>
+        <v>./test-results/Kanban Information.jpg</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f>CONCATENATE("{test:'",C2,"',url :'",D2,"', page_title:'",E2,"',page_heading:'",F2,"',screenshot_path:'",G2,"'},")</f>
+        <v>{test:'Card Information 1',url :'http://localhost:8000/card_information/1/', page_title:'Kanban Information 1',page_heading:'Kanban Information',screenshot_path:'./test-results/Kanban Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f t="shared" ref="G3:G28" si="0">CONCATENATE("./test-results/",F3,".jpg")</f>
+        <v>./test-results/Change Task.jpg</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <f t="shared" ref="H3:H28" si="1">CONCATENATE("{test:'",C3,"',url :'",D3,"', page_title:'",E3,"',page_heading:'",F3,"',screenshot_path:'",G3,"'},")</f>
+        <v>{test:'Change Task Information 1',url :'http://localhost:8000/change_task_information/1/', page_title:'Change Task 1',page_heading:'Change Task',screenshot_path:'./test-results/Change Task.jpg'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Customer Information.jpg</v>
+      </c>
+      <c r="H4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Customer Information 1',url :'http://localhost:8000/customer_information/1/', page_title:'Customer Information 1',page_heading:'Customer Information',screenshot_path:'./test-results/Customer Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="G5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Group Information.jpg</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Group Information 1',url :'http://localhost:8000/group_information/1/', page_title:'Group Information 1',page_heading:'Group Information',screenshot_path:'./test-results/Group Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="G6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Kanban Information.jpg</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Kanban Information 1',url :'http://localhost:8000/kanban_information/1/', page_title:'Kanban Information 1',page_heading:'Kanban Information',screenshot_path:'./test-results/Kanban Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="G7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Kanban Information.jpg</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Kanban Card Information 1',url :'http://localhost:8000/kanban_information/1/card/1/', page_title:'Kanban Information 1',page_heading:'Kanban Information',screenshot_path:'./test-results/Kanban Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Kanban Information.jpg</v>
+      </c>
+      <c r="H8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Kanban Information Edit Board 1',url :'http://localhost:8000/kanban_information/1/edit_board/', page_title:'Kanban Information 1',page_heading:'Kanban Information',screenshot_path:'./test-results/Kanban Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="G9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Group.jpg</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Group',url :'http://localhost:8000/new_group/', page_title:'New Group',page_heading:'New Group',screenshot_path:'./test-results/New Group.jpg'},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="G10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Kanban.jpg</v>
+      </c>
+      <c r="H10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Kanban',url :'http://localhost:8000/new_kanban/', page_title:'New Kanban',page_heading:'New Kanban',screenshot_path:'./test-results/New Kanban.jpg'},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="G11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Organisation.jpg</v>
+      </c>
+      <c r="H11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Organisation',url :'http://localhost:8000/new_organisation/', page_title:'New Organisation',page_heading:'New Organisation',screenshot_path:'./test-results/New Organisation.jpg'},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="G12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Permission Set.jpg</v>
+      </c>
+      <c r="H12" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Permission Set',url :'http://localhost:8000/new_permission_set/', page_title:'New Permission Set',page_heading:'New Permission Set',screenshot_path:'./test-results/New Permission Set.jpg'},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="G13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Project.jpg</v>
+      </c>
+      <c r="H13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Project',url :'http://localhost:8000/new_project/', page_title:'New Project',page_heading:'New Project',screenshot_path:'./test-results/New Project.jpg'},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="G14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Request for Change.jpg</v>
+      </c>
+      <c r="H14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Request for Change',url :'http://localhost:8000/new_request_for_change/', page_title:'New Request for Change',page_heading:'New Request for Change',screenshot_path:'./test-results/New Request for Change.jpg'},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="G15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Requirement Item.jpg</v>
+      </c>
+      <c r="H15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Requirement Item',url :'http://localhost:8000/new_requirement_item/save/1/', page_title:'New Requirement Item',page_heading:'New Requirement Item',screenshot_path:'./test-results/New Requirement Item.jpg'},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="G16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Requirement.jpg</v>
+      </c>
+      <c r="H16" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Requirement',url :'http://localhost:8000/new_requirement/', page_title:'New Requirement',page_heading:'New Requirement',screenshot_path:'./test-results/New Requirement.jpg'},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="G17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New Task.jpg</v>
+      </c>
+      <c r="H17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New Task',url :'http://localhost:8000/new_task/', page_title:'New Task',page_heading:'New Task',screenshot_path:'./test-results/New Task.jpg'},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="G18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/New User.jpg</v>
+      </c>
+      <c r="H18" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'New User',url :'http://localhost:8000/new_user/', page_title:'New User',page_heading:'New User',screenshot_path:'./test-results/New User.jpg'},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="G19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Organisation Information.jpg</v>
+      </c>
+      <c r="H19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Organisation Information 1',url :'http://localhost:8000/organisation_information/1/', page_title:'Organisation Information 1',page_heading:'Organisation Information',screenshot_path:'./test-results/Organisation Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="G20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Permission Set Information.jpg</v>
+      </c>
+      <c r="H20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Permission Set Information 1',url :'http://localhost:8000/permission_set_information/1/', page_title:'Permission Set Information 1',page_heading:'Permission Set Information',screenshot_path:'./test-results/Permission Set Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Profile Information.jpg</v>
+      </c>
+      <c r="H21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Profile Information',url :'http://localhost:8000/profile_information/', page_title:'Profile Information',page_heading:'Profile Information',screenshot_path:'./test-results/Profile Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="G22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Project Information.jpg</v>
+      </c>
+      <c r="H22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Project Information 1',url :'http://localhost:8000/project_information/1/', page_title:'Project Information 1',page_heading:'Project Information',screenshot_path:'./test-results/Project Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="G23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Requirement Information.jpg</v>
+      </c>
+      <c r="H23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Requirement Information 1',url :'http://localhost:8000/requirement_information/1/', page_title:'Requirement Information 1',page_heading:'Requirement Information',screenshot_path:'./test-results/Requirement Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="G24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Requirement Item Information.jpg</v>
+      </c>
+      <c r="H24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Requirement Item Information 1',url :'http://localhost:8000/requirement_item_information/1/', page_title:'Requirement Item Information 1',page_heading:'Requirement Item Information',screenshot_path:'./test-results/Requirement Item Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="G25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/RFC Information.jpg</v>
+      </c>
+      <c r="H25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'RFC Information 1',url :'http://localhost:8000/rfc_information/1/', page_title:'RFC Information 1',page_heading:'RFC Information',screenshot_path:'./test-results/RFC Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="G26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Search.jpg</v>
+      </c>
+      <c r="H26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Search',url :'http://localhost:8000/search/', page_title:'Search',page_heading:'Search',screenshot_path:'./test-results/Search.jpg'},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="G27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/Task Information.jpg</v>
+      </c>
+      <c r="H27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'Task Information 1',url :'http://localhost:8000/task_information/1/', page_title:'Task Information 1',page_heading:'Task Information',screenshot_path:'./test-results/Task Information.jpg'},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="G28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>./test-results/User Information.jpg</v>
+      </c>
+      <c r="H28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>{test:'User Information 1',url :'http://localhost:8000/user_information/1/', page_title:'User Information 1',page_heading:'User Information',screenshot_path:'./test-results/User Information.jpg'},</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2:B28" r:id="rId1" display="http://localhost:8000/" xr:uid="{B975EB6F-144D-7043-AE2A-4878C54F8F3D}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{4DE8A32F-EC3C-A941-AAE7-16765B6F295E}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{C830F079-0096-6848-8C2C-DF82A432E231}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{AF8D53AA-4BC3-3E4E-96E2-F08E7BB9784F}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{20E5028B-7FC5-1B44-8EEA-4DD035444B31}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{8EE0EE0F-5FFC-B849-B606-63CA1E79F77E}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{49C8DDE5-BEF2-EC4D-900D-1C97C3CF8181}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{2833A023-F98F-C046-A9FC-0C4F0C66D083}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{0E425A39-5AF8-DE46-9B0A-CCED572F75F2}"/>
+    <hyperlink ref="D19" r:id="rId10" xr:uid="{C9234A53-73D7-084E-8008-6497A53EA55F}"/>
+    <hyperlink ref="D20" r:id="rId11" xr:uid="{A0E380FD-6B71-4B47-B500-4D753BA1FD42}"/>
+    <hyperlink ref="D22" r:id="rId12" xr:uid="{BBF34489-551D-934F-8624-581A7CB3CA98}"/>
+    <hyperlink ref="D23" r:id="rId13" xr:uid="{45D39302-948F-8248-AD4B-53A2C79BFBE8}"/>
+    <hyperlink ref="D24" r:id="rId14" xr:uid="{797778A4-F939-BC4E-83EC-6CE00324CE51}"/>
+    <hyperlink ref="D25" r:id="rId15" xr:uid="{FBA68E1E-DCFE-1F45-94C9-DE200C300D4F}"/>
+    <hyperlink ref="D27" r:id="rId16" xr:uid="{B8BD1E72-0349-3B41-B918-7287C94F95C2}"/>
+    <hyperlink ref="D28" r:id="rId17" xr:uid="{814C3E65-676D-2340-A8AA-AFD728296DBD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to the template of unit tests spread sheet
</commit_message>
<xml_diff>
--- a/NearBeach/tests/Template of Unit Tests.xlsx
+++ b/NearBeach/tests/Template of Unit Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke/Sites/NearBeach/NearBeach/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5386CDB-1D71-3E41-9991-16B3609A444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AD8F92-74F4-6F4F-8074-CA355FE63BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{49CA0490-8A4C-AD4D-8E45-19DFC0D521BF}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{49CA0490-8A4C-AD4D-8E45-19DFC0D521BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Data" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="678">
   <si>
     <t>AddBugForm</t>
   </si>
@@ -2045,9 +2045,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Change Task</t>
-  </si>
-  <si>
     <t>Customer Information</t>
   </si>
   <si>
@@ -2073,6 +2070,12 @@
   </si>
   <si>
     <t>User Information</t>
+  </si>
+  <si>
+    <t>Kanban Admin Only</t>
+  </si>
+  <si>
+    <t>Change Task - 1</t>
   </si>
 </sst>
 </file>
@@ -8348,7 +8351,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8357,7 +8360,8 @@
     <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="84.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="193.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -8405,15 +8409,15 @@
         <v>613</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>CONCATENATE("./test-results/",F2,".jpg")</f>
-        <v>./test-results/Kanban Information.jpg</v>
+        <v>./test-results/Kanban Admin Only.jpg</v>
       </c>
       <c r="H2" s="3" t="str">
         <f>CONCATENATE("{test:'",C2,"',url :'",D2,"', page_title:'",E2,"',page_heading:'",F2,"',screenshot_path:'",G2,"'},")</f>
-        <v>{test:'Card Information 1',url :'http://localhost:8000/card_information/1/', page_title:'Kanban Information 1',page_heading:'Kanban Information',screenshot_path:'./test-results/Kanban Information.jpg'},</v>
+        <v>{test:'Card Information 1',url :'http://localhost:8000/card_information/1/', page_title:'Kanban Information 1',page_heading:'Kanban Admin Only',screenshot_path:'./test-results/Kanban Admin Only.jpg'},</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -8433,15 +8437,15 @@
         <v>664</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" ref="G3:G28" si="0">CONCATENATE("./test-results/",F3,".jpg")</f>
-        <v>./test-results/Change Task.jpg</v>
+        <v>./test-results/Change Task - 1.jpg</v>
       </c>
       <c r="H3" s="3" t="str">
         <f t="shared" ref="H3:H28" si="1">CONCATENATE("{test:'",C3,"',url :'",D3,"', page_title:'",E3,"',page_heading:'",F3,"',screenshot_path:'",G3,"'},")</f>
-        <v>{test:'Change Task Information 1',url :'http://localhost:8000/change_task_information/1/', page_title:'Change Task 1',page_heading:'Change Task',screenshot_path:'./test-results/Change Task.jpg'},</v>
+        <v>{test:'Change Task Information 1',url :'http://localhost:8000/change_task_information/1/', page_title:'Change Task 1',page_heading:'Change Task - 1',screenshot_path:'./test-results/Change Task - 1.jpg'},</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -8461,7 +8465,7 @@
         <v>611</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -8489,7 +8493,7 @@
         <v>612</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -8545,15 +8549,15 @@
         <v>613</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>./test-results/Kanban Information.jpg</v>
+        <v>./test-results/Kanban Admin Only.jpg</v>
       </c>
       <c r="H7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>{test:'Kanban Card Information 1',url :'http://localhost:8000/kanban_information/1/card/1/', page_title:'Kanban Information 1',page_heading:'Kanban Information',screenshot_path:'./test-results/Kanban Information.jpg'},</v>
+        <v>{test:'Kanban Card Information 1',url :'http://localhost:8000/kanban_information/1/card/1/', page_title:'Kanban Information 1',page_heading:'Kanban Admin Only',screenshot_path:'./test-results/Kanban Admin Only.jpg'},</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -8573,15 +8577,15 @@
         <v>613</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>./test-results/Kanban Information.jpg</v>
+        <v>./test-results/Kanban Admin Only.jpg</v>
       </c>
       <c r="H8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>{test:'Kanban Information Edit Board 1',url :'http://localhost:8000/kanban_information/1/edit_board/', page_title:'Kanban Information 1',page_heading:'Kanban Information',screenshot_path:'./test-results/Kanban Information.jpg'},</v>
+        <v>{test:'Kanban Information Edit Board 1',url :'http://localhost:8000/kanban_information/1/edit_board/', page_title:'Kanban Information 1',page_heading:'Kanban Admin Only',screenshot_path:'./test-results/Kanban Admin Only.jpg'},</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -8909,7 +8913,7 @@
         <v>628</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -8965,7 +8969,7 @@
         <v>630</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -8993,7 +8997,7 @@
         <v>631</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -9021,7 +9025,7 @@
         <v>632</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -9049,7 +9053,7 @@
         <v>633</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -9105,7 +9109,7 @@
         <v>635</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -9133,7 +9137,7 @@
         <v>636</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>